<commit_message>
added fixes after review
</commit_message>
<xml_diff>
--- a/mshik/lesson_6/data/users.xlsx
+++ b/mshik/lesson_6/data/users.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,44 +436,62 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>Person1</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>Person2</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>phone_number</t>
+          <t>Person3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Person4</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Person5</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="n">
-        <v>0</v>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>12345</v>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Maxim</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>+375(44)2425340</t>
-        </is>
+      <c r="C2" t="n">
+        <v>123456</v>
+      </c>
+      <c r="D2" t="n">
+        <v>234567</v>
+      </c>
+      <c r="E2" t="n">
+        <v>345678</v>
+      </c>
+      <c r="F2" t="n">
+        <v>456789</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="B3" t="n">
-        <v>123456</v>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Maxim</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
@@ -482,61 +500,49 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>+375(44)5384644</t>
+          <t>Alex</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Yura</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="n">
-        <v>234567</v>
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>phone</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>+375(44)6040934</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Alex</t>
+          <t>+375(44)9500689</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>+375(44)4105082</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="n">
-        <v>345678</v>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Adam</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>+375(44)3665023</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="n">
-        <v>456789</v>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Yura</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>+375(44)1383588</t>
+          <t>+375(44)7701371</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>+375(44)4560025</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>+375(44)2833246</t>
         </is>
       </c>
     </row>

</xml_diff>